<commit_message>
Replaced USB A with micro USB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABEACE02ECA00B1F559C5ADE5898" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{590DD3B9-AE6D-460A-88F8-0DDCB099E324}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="11_F25DC773A252ABEACE02ECA00B1F559C5ADE5898" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{94BC7B23-4314-47E5-83A6-5EAB1D64F4A9}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="21525" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Vendor</t>
   </si>
@@ -116,24 +115,6 @@
     <t>Voltage Reg</t>
   </si>
   <si>
-    <t>AE11187-ND</t>
-  </si>
-  <si>
-    <t>Assmann WSW</t>
-  </si>
-  <si>
-    <t>SMT Horizontal</t>
-  </si>
-  <si>
-    <t>USB Type A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/assmann-wsw-components/AU-Y1006-2/AE11187-ND/5031761</t>
-  </si>
-  <si>
-    <t>http://www.assmann-wsw.com/fileadmin/datasheets/ASS_5774_CO.pdf</t>
-  </si>
-  <si>
     <t>36-92-ND</t>
   </si>
   <si>
@@ -149,12 +130,6 @@
     <t>https://www.digikey.com/product-detail/en/keystone-electronics/92/36-92-ND/82326</t>
   </si>
   <si>
-    <t>27pF Capacitor</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/500R07S270GV4T/712-1276-1-ND/1786738</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/yageo/RC0402FR-0722RL/311-22.0LRCT-ND/729509</t>
   </si>
   <si>
@@ -210,6 +185,51 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-2AEB3480X/P348DCCT-ND/3063784</t>
+  </si>
+  <si>
+    <t>Micro USB Type B</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/amphenol-icc-fci/10103592-0001LF/609-4048-1-ND/2350355</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-icc.com/media/wysiwyg/files/documentation/datasheet/inputoutput/io_usb_micro.pdf</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>609-4048-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM31CD80J107ME39L/490-10525-1-ND/5026461</t>
+  </si>
+  <si>
+    <t>100uF Capacitor</t>
+  </si>
+  <si>
+    <t>490-10525-1-ND</t>
+  </si>
+  <si>
+    <t>Muramata</t>
+  </si>
+  <si>
+    <t>GRM31CD80J107ME39L</t>
+  </si>
+  <si>
+    <t>22pF Capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/avx-corporation/04025A220FAT2A/478-5765-1-ND/2136357</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>478-5765-1-ND</t>
+  </si>
+  <si>
+    <t>04025A220FAT2A</t>
   </si>
 </sst>
 </file>
@@ -219,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,12 +256,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="4"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -255,12 +269,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -300,38 +308,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,22 +673,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.29296875" customWidth="1"/>
-    <col min="3" max="3" width="14.29296875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="10" max="10" width="9.1171875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="125.5703125" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,88 +724,92 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>0.99</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <f>H2*G2</f>
         <v>0.99</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="E3">
+      <c r="C3" s="7"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
         <v>603</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>0.22</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I15" si="0">H3*G3</f>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I16" si="0">H3*G3</f>
         <v>0.44</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>0.27</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
@@ -804,275 +820,378 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>1.41</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <f t="shared" si="0"/>
         <v>1.41</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I7" si="1">G6*H6</f>
+        <v>0.78</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D7" s="4">
+        <v>92</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.82</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I7" si="1">G6*H6</f>
-        <v>0.82</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7">
-        <v>92</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>8</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>0.32</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <f t="shared" si="1"/>
         <v>2.56</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="I8">
+        <v>33</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1206</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="4">
+        <v>402</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="4">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="I9">
+      <c r="J11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="4">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="I10">
+      <c r="J12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="I11">
+      <c r="J13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4">
+        <v>4</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="I12">
+      <c r="J14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="I13">
+      <c r="J15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="4">
+        <v>2</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="172" x14ac:dyDescent="0.5">
-      <c r="A16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="9">
-        <v>1</v>
-      </c>
-      <c r="H16" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="I16" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>4.2</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="K18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1082,18 +1201,20 @@
     <hyperlink ref="J2" r:id="rId4" xr:uid="{BE8BFA7B-A934-4AB8-900A-3634C5EB9A7F}"/>
     <hyperlink ref="J4" r:id="rId5" xr:uid="{382DE541-6CA8-49E7-A820-77EC810D5C40}"/>
     <hyperlink ref="J5" r:id="rId6" xr:uid="{D20EF60C-ADAE-4C03-8533-08B7BB61A105}"/>
-    <hyperlink ref="J6" r:id="rId7" xr:uid="{AF6576AF-D2FB-429F-85DA-C48DE43342E6}"/>
-    <hyperlink ref="J16" r:id="rId8" xr:uid="{56377A12-5C9F-4227-AFE6-E52B59DD89F5}"/>
-    <hyperlink ref="J17" r:id="rId9" xr:uid="{9D6BEF5C-EB14-484F-9009-1F20D1097075}"/>
-    <hyperlink ref="J9" r:id="rId10" xr:uid="{B0FF7F06-0974-4894-B555-D710DC25E825}"/>
-    <hyperlink ref="J10" r:id="rId11" xr:uid="{2E96E0BF-AEB7-4F25-81FB-52DBB73363BC}"/>
-    <hyperlink ref="J11" r:id="rId12" xr:uid="{80C08C64-CDFF-4CBA-96DA-1F01904053DA}"/>
-    <hyperlink ref="J12" r:id="rId13" xr:uid="{A1E72ADD-C0E6-48EA-93C5-19DC50D2134E}"/>
-    <hyperlink ref="J13" r:id="rId14" xr:uid="{94D99EE2-BB36-4057-9F79-FFF008589F89}"/>
-    <hyperlink ref="J14" r:id="rId15" xr:uid="{65048888-69CC-4833-A7AB-77A6FBB6F593}"/>
+    <hyperlink ref="J11" r:id="rId7" xr:uid="{2E96E0BF-AEB7-4F25-81FB-52DBB73363BC}"/>
+    <hyperlink ref="J12" r:id="rId8" xr:uid="{80C08C64-CDFF-4CBA-96DA-1F01904053DA}"/>
+    <hyperlink ref="J13" r:id="rId9" xr:uid="{A1E72ADD-C0E6-48EA-93C5-19DC50D2134E}"/>
+    <hyperlink ref="J14" r:id="rId10" xr:uid="{94D99EE2-BB36-4057-9F79-FFF008589F89}"/>
+    <hyperlink ref="J15" r:id="rId11" xr:uid="{65048888-69CC-4833-A7AB-77A6FBB6F593}"/>
+    <hyperlink ref="J6" r:id="rId12" xr:uid="{DF06F925-0B32-4DA5-B08C-54C9220DDC3E}"/>
+    <hyperlink ref="K6" r:id="rId13" xr:uid="{6A5D0A54-082B-4E77-B9C5-2D2A29522F28}"/>
+    <hyperlink ref="J9" r:id="rId14" xr:uid="{7A24AC0E-27AB-492F-B475-002394AAE526}"/>
+    <hyperlink ref="J10" r:id="rId15" xr:uid="{A7BB5DCB-0F25-4A0E-A5B6-8FF86ED3A88A}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{9D6BEF5C-EB14-484F-9009-1F20D1097075}"/>
+    <hyperlink ref="J17" r:id="rId17" xr:uid="{56377A12-5C9F-4227-AFE6-E52B59DD89F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -1102,10 +1223,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>